<commit_message>
Delete some information from first page
</commit_message>
<xml_diff>
--- a/Checklists/Forms.xlsx
+++ b/Checklists/Forms.xlsx
@@ -558,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,31 +650,6 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>